<commit_message>
update dataset_description & add review docx
</commit_message>
<xml_diff>
--- a/data/dataset_description.xlsx
+++ b/data/dataset_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antimo.Musone\OneDrive - EY\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbpr/GitHub/Acea-Smart-Water-Analytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{E5049B6C-83BA-4CA2-BCA6-803F3D3D2FB8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{92A4E9FD-68F0-4407-91AC-8B3B8B8CAB75}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE19F36-2BAE-7249-907E-F1156A38E762}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7000" yWindow="1140" windowWidth="22240" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets_Description" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="131">
   <si>
     <t>Database</t>
   </si>
@@ -926,13 +926,29 @@
   </si>
   <si>
     <t>Depth_to_Groundwater_Y ( only in this case it's the height above the sensor)</t>
+  </si>
+  <si>
+    <t>water spring</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>aquifer</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>river</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>lake</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -966,6 +982,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Wawati TC"/>
+      <family val="3"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1077,7 +1099,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1098,28 +1120,59 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="一般" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1145,10 +1198,10 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table2511" displayName="Table2511" ref="A12:C17" totalsRowShown="0">
-  <autoFilter ref="A12:C17" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table2511" displayName="Table2511" ref="A13:C18" totalsRowShown="0">
+  <autoFilter ref="A13:C18" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Field"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Field" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Format"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Description"/>
   </tableColumns>
@@ -1157,8 +1210,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Table3612" displayName="Table3612" ref="G13:H17" totalsRowShown="0">
-  <autoFilter ref="G13:H17" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Table3612" displayName="Table3612" ref="G14:H18" totalsRowShown="0">
+  <autoFilter ref="G14:H18" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Code"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Values"/>
@@ -1168,8 +1221,8 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table361214" displayName="Table361214" ref="G22:H27" totalsRowShown="0">
-  <autoFilter ref="G22:H27" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table361214" displayName="Table361214" ref="G23:H28" totalsRowShown="0">
+  <autoFilter ref="G23:H28" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Code"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Values"/>
@@ -1179,10 +1232,10 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table251115" displayName="Table251115" ref="A21:C27" totalsRowShown="0">
-  <autoFilter ref="A21:C27" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table251115" displayName="Table251115" ref="A22:C28" totalsRowShown="0">
+  <autoFilter ref="A22:C28" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Field"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Field" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Format"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Description"/>
   </tableColumns>
@@ -1191,8 +1244,8 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table36121420" displayName="Table36121420" ref="G32:H36" totalsRowShown="0">
-  <autoFilter ref="G32:H36" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table36121420" displayName="Table36121420" ref="G33:H37" totalsRowShown="0">
+  <autoFilter ref="G33:H37" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Code"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Values"/>
@@ -1202,10 +1255,10 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table25111521" displayName="Table25111521" ref="A31:C36" totalsRowShown="0">
-  <autoFilter ref="A31:C36" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table25111521" displayName="Table25111521" ref="A32:C37" totalsRowShown="0">
+  <autoFilter ref="A32:C37" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="Field"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="Field" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="Format"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="Description"/>
   </tableColumns>
@@ -1214,10 +1267,10 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table257923" displayName="Table257923" ref="A67:C70" totalsRowShown="0">
-  <autoFilter ref="A67:C70" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table257923" displayName="Table257923" ref="A68:C71" totalsRowShown="0">
+  <autoFilter ref="A68:C71" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="Field"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="Field" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="Format"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="Description"/>
   </tableColumns>
@@ -1226,8 +1279,8 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table3681024" displayName="Table3681024" ref="G68:H70" totalsRowShown="0">
-  <autoFilter ref="G68:H70" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table3681024" displayName="Table3681024" ref="G69:H71" totalsRowShown="0">
+  <autoFilter ref="G69:H71" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="Code"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="Values"/>
@@ -1237,10 +1290,10 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Table25792325" displayName="Table25792325" ref="A74:C78" totalsRowShown="0">
-  <autoFilter ref="A74:C78" xr:uid="{00000000-0009-0000-0100-000012000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Table25792325" displayName="Table25792325" ref="A75:C79" totalsRowShown="0">
+  <autoFilter ref="A75:C79" xr:uid="{00000000-0009-0000-0100-000012000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="Field"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="Field" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="Format"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="Description"/>
   </tableColumns>
@@ -1249,8 +1302,8 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="Table368102426" displayName="Table368102426" ref="G75:H78" totalsRowShown="0">
-  <autoFilter ref="G75:H78" xr:uid="{00000000-0009-0000-0100-000013000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="Table368102426" displayName="Table368102426" ref="G76:H79" totalsRowShown="0">
+  <autoFilter ref="G76:H79" xr:uid="{00000000-0009-0000-0100-000013000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="Code"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="Values"/>
@@ -1260,10 +1313,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A2:C8" totalsRowShown="0">
-  <autoFilter ref="A2:C8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A3:C9" totalsRowShown="0">
+  <autoFilter ref="A3:C9" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Field"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Field" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Format"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description"/>
   </tableColumns>
@@ -1272,8 +1325,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="G3:H8" totalsRowShown="0">
-  <autoFilter ref="G3:H8" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="G4:H9" totalsRowShown="0">
+  <autoFilter ref="G4:H9" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Code"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Values"/>
@@ -1283,10 +1336,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table25" displayName="Table25" ref="A41:C46" totalsRowShown="0">
-  <autoFilter ref="A41:C46" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table25" displayName="Table25" ref="A42:C47" totalsRowShown="0">
+  <autoFilter ref="A42:C47" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Field"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Field" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Format"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Description"/>
   </tableColumns>
@@ -1295,8 +1348,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table36" displayName="Table36" ref="G42:H46" totalsRowShown="0">
-  <autoFilter ref="G42:H46" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table36" displayName="Table36" ref="G43:H47" totalsRowShown="0">
+  <autoFilter ref="G43:H47" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Code"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Values"/>
@@ -1306,10 +1359,10 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table257" displayName="Table257" ref="A50:C54" totalsRowShown="0">
-  <autoFilter ref="A50:C54" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table257" displayName="Table257" ref="A51:C55" totalsRowShown="0">
+  <autoFilter ref="A51:C55" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Field"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Field" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Format"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Description"/>
   </tableColumns>
@@ -1318,8 +1371,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table368" displayName="Table368" ref="G51:H54" totalsRowShown="0">
-  <autoFilter ref="G51:H54" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table368" displayName="Table368" ref="G52:H55" totalsRowShown="0">
+  <autoFilter ref="G52:H55" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Code"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Values"/>
@@ -1329,10 +1382,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table2579" displayName="Table2579" ref="A58:C63" totalsRowShown="0">
-  <autoFilter ref="A58:C63" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table2579" displayName="Table2579" ref="A59:C64" totalsRowShown="0">
+  <autoFilter ref="A59:C64" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Field"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Field" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Format"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Description"/>
   </tableColumns>
@@ -1341,8 +1394,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table36810" displayName="Table36810" ref="G59:H61" totalsRowShown="0">
-  <autoFilter ref="G59:H61" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table36810" displayName="Table36810" ref="G60:H62" totalsRowShown="0">
+  <autoFilter ref="G60:H62" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Code"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Values"/>
@@ -1352,7 +1405,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1650,20 +1703,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="146.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="10.44140625" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" customWidth="1"/>
+    <col min="4" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1674,7 +1727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1685,7 +1738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1696,7 +1749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1707,7 +1760,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1718,7 +1771,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1729,7 +1782,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1740,7 +1793,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -1751,7 +1804,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1760,7 +1813,7 @@
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1770,6 +1823,7 @@
       <c r="C10" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <tableParts count="1">
@@ -1780,1039 +1834,1073 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O79"/>
+  <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="102.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.88671875" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="102.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" customWidth="1"/>
+    <col min="15" max="15" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>57</v>
+    <row r="10" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>63</v>
+    <row r="19" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G28" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>71</v>
+    <row r="29" spans="1:8" s="7" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>76</v>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" s="7" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="G47" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
+    <row r="48" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="H52" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G54" s="4" t="s">
+      <c r="G55" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="H55" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
+    <row r="56" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G59" s="1" t="s">
+      <c r="G60" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H59" s="1" t="s">
+      <c r="H60" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="6"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="6"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
+    <row r="65" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A68" s="4" t="s">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G68" s="1" t="s">
+      <c r="G69" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H68" s="1" t="s">
+      <c r="H69" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G70" s="4" t="s">
+      <c r="G71" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H70" s="1" t="s">
+      <c r="H71" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A73" s="3" t="s">
+    <row r="72" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C75" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A75" s="4" t="s">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G75" s="1" t="s">
+      <c r="G76" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H75" s="1" t="s">
+      <c r="H76" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G76" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H77" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H77" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G78" s="4" t="s">
+      <c r="G79" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H78" s="1" t="s">
+      <c r="H79" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <tableParts count="18">
@@ -2842,20 +2930,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F2B66A-E66D-4374-BE1D-2D7BB57A9E13}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" customWidth="1"/>
-    <col min="4" max="4" width="24.5546875" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>124</v>
       </c>
@@ -2872,25 +2960,25 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
+      <c r="E2" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="16"/>
       <c r="B3" s="9" t="s">
         <v>113</v>
       </c>
@@ -2900,12 +2988,12 @@
       <c r="D3" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
+      <c r="E3" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="16"/>
       <c r="B4" s="9" t="s">
         <v>114</v>
       </c>
@@ -2915,12 +3003,12 @@
       <c r="D4" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
       <c r="B5" s="9" t="s">
         <v>115</v>
       </c>
@@ -2930,27 +3018,27 @@
       <c r="D5" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16" t="s">
+      <c r="E5" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="17"/>
+      <c r="B6" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="E6" s="17" t="s">
+      <c r="C6" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
         <v>57</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -2962,13 +3050,13 @@
       <c r="D7" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="18" t="s">
+      <c r="E7" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="16"/>
+      <c r="B8" s="15" t="s">
         <v>126</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -2977,12 +3065,12 @@
       <c r="D8" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
+      <c r="E8" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="16"/>
       <c r="B9" s="9" t="s">
         <v>114</v>
       </c>
@@ -2992,27 +3080,27 @@
       <c r="D9" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="17"/>
+      <c r="B10" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" s="16" t="s">
+      <c r="C10" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+      <c r="E10" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -3024,12 +3112,12 @@
       <c r="D11" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
+      <c r="E11" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="16"/>
       <c r="B12" s="9" t="s">
         <v>113</v>
       </c>
@@ -3039,12 +3127,12 @@
       <c r="D12" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
+      <c r="E12" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="16"/>
       <c r="B13" s="9" t="s">
         <v>114</v>
       </c>
@@ -3054,12 +3142,12 @@
       <c r="D13" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="16"/>
       <c r="B14" s="9" t="s">
         <v>117</v>
       </c>
@@ -3069,27 +3157,27 @@
       <c r="D14" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E14" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16" t="s">
+      <c r="E14" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="17"/>
+      <c r="B15" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" s="17" t="s">
+      <c r="C15" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
         <v>71</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -3101,12 +3189,12 @@
       <c r="D16" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
+      <c r="E16" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="16"/>
       <c r="B17" s="9" t="s">
         <v>113</v>
       </c>
@@ -3116,12 +3204,12 @@
       <c r="D17" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
+      <c r="E17" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="16"/>
       <c r="B18" s="9" t="s">
         <v>114</v>
       </c>
@@ -3131,27 +3219,27 @@
       <c r="D18" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="17"/>
+      <c r="B19" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
+      <c r="D19" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="16" t="s">
         <v>76</v>
       </c>
       <c r="B20" s="9" t="s">
@@ -3163,12 +3251,12 @@
       <c r="D20" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
+      <c r="E20" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="16"/>
       <c r="B21" s="9" t="s">
         <v>113</v>
       </c>
@@ -3178,12 +3266,12 @@
       <c r="D21" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
+      <c r="E21" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="16"/>
       <c r="B22" s="9" t="s">
         <v>114</v>
       </c>
@@ -3193,27 +3281,27 @@
       <c r="D22" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="17"/>
+      <c r="B23" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D23" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
+      <c r="D23" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
         <v>83</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -3225,12 +3313,12 @@
       <c r="D24" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E24" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
+      <c r="E24" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="16"/>
       <c r="B25" s="9" t="s">
         <v>120</v>
       </c>
@@ -3240,27 +3328,27 @@
       <c r="D25" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
-      <c r="B26" s="16" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="17"/>
+      <c r="B26" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="C26" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="E26" s="17" t="s">
+      <c r="C26" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
         <v>91</v>
       </c>
       <c r="B27" s="9" t="s">
@@ -3272,12 +3360,12 @@
       <c r="D27" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E27" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
+      <c r="E27" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="16"/>
       <c r="B28" s="9" t="s">
         <v>120</v>
       </c>
@@ -3287,12 +3375,12 @@
       <c r="D28" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="16"/>
       <c r="B29" s="9" t="s">
         <v>94</v>
       </c>
@@ -3302,27 +3390,27 @@
       <c r="D29" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E29" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="15"/>
-      <c r="B30" s="16" t="s">
+      <c r="E29" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="17"/>
+      <c r="B30" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="D30" s="16" t="s">
+      <c r="C30" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="E30" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="13" t="s">
+      <c r="E30" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
         <v>98</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -3334,27 +3422,27 @@
       <c r="D31" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E31" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
-      <c r="B32" s="16" t="s">
+      <c r="E31" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="17"/>
+      <c r="B32" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D32" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="13" t="s">
+      <c r="D32" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="16" t="s">
         <v>125</v>
       </c>
       <c r="B33" s="9" t="s">
@@ -3366,12 +3454,12 @@
       <c r="D33" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="13"/>
+      <c r="E33" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="16"/>
       <c r="B34" s="9" t="s">
         <v>120</v>
       </c>
@@ -3381,44 +3469,60 @@
       <c r="D34" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="17"/>
+      <c r="B35" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="C35" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="D35" s="16" t="s">
+      <c r="C35" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E35" s="14" t="s">
         <v>111</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E35" xr:uid="{E8622992-0D0A-4D32-8E75-964F2015A4FB}"/>
   <mergeCells count="9">
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A15"/>
     <mergeCell ref="A16:A19"/>
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A15"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A2CE81D0E9067B4C9491F29EF2260D9A" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5b5f5cf789d994f288cb530aae4d4947">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1ee2afc6-efc0-4dcc-be09-aabefb754106" xmlns:ns4="6dff4707-7bf8-4102-b125-42e04ae9fdfc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86a904f73a016299fbde656704a2a3dc" ns3:_="" ns4:_="">
     <xsd:import namespace="1ee2afc6-efc0-4dcc-be09-aabefb754106"/>
@@ -3641,36 +3745,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8A7265-CDBA-4BB3-9DDC-8912F09875BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3C7A22F-15D8-4BE7-82F0-4B9B46CEAC3F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1ee2afc6-efc0-4dcc-be09-aabefb754106"/>
-    <ds:schemaRef ds:uri="6dff4707-7bf8-4102-b125-42e04ae9fdfc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3693,9 +3771,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3C7A22F-15D8-4BE7-82F0-4B9B46CEAC3F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8A7265-CDBA-4BB3-9DDC-8912F09875BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1ee2afc6-efc0-4dcc-be09-aabefb754106"/>
+    <ds:schemaRef ds:uri="6dff4707-7bf8-4102-b125-42e04ae9fdfc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>